<commit_message>
moving to github pt2
</commit_message>
<xml_diff>
--- a/data-raw/cpi/cpi_2011.xlsx
+++ b/data-raw/cpi/cpi_2011.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desk\google_drive\research\_packages\ipsed\data-raw\cpi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F446B2AC-8149-4187-9FC8-8513C4E5BDD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{35F7BAE0-710E-40FF-A3D5-48F687BCB49F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="-120" windowWidth="28050" windowHeight="16440" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="870" yWindow="-120" windowWidth="28050" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="take1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -25,20 +25,20 @@
     <sheet name="2009 raw" sheetId="10" state="hidden" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="boostrap">#REF!</definedName>
     <definedName name="_CPI2010">#REF!</definedName>
     <definedName name="_CPI2011">#REF!</definedName>
     <definedName name="_raw2009">'2009 raw'!$A$2:$S$212</definedName>
+    <definedName name="boostrap">#REF!</definedName>
     <definedName name="take1">take1!$A$2:$S$184</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="Aidan Brown - Personal View" guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" mergeInterval="0" personalView="1" maximized="1" xWindow="58" yWindow="-8" windowWidth="1870" windowHeight="1096" activeSheetId="2"/>
     <customWorkbookView name="efichtl - Personal View" guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1881" windowHeight="898" activeSheetId="8"/>
     <customWorkbookView name="Note - Personal View" guid="{7279341D-4A93-45C7-96BD-49257ECF5365}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1788" windowHeight="973" activeSheetId="2"/>
     <customWorkbookView name="severett - Personal View" guid="{D1F0CD4F-E178-400D-8129-E15FD202F118}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1788" windowHeight="973" activeSheetId="2"/>
     <customWorkbookView name="adashwood - Personal View" guid="{62F7D542-8BF7-4494-AF3C-DE037CC9A023}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="885" activeSheetId="2"/>
     <customWorkbookView name="Thomas Coombes - Personal View" guid="{74EB1777-F5EA-4A6C-95F8-C57AD2099046}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" activeSheetId="2"/>
+    <customWorkbookView name="Aidan Brown - Personal View" guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" mergeInterval="0" personalView="1" maximized="1" xWindow="58" yWindow="-8" windowWidth="1870" windowHeight="1096" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -55,13 +55,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dr. Johann Graf Lambsdorff</author>
     <author>Note</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" guid="{4F15D710-3AC6-4E6B-BE37-A261185AE67A}" shapeId="0">
+    <comment ref="D1" authorId="0" guid="{A62510E4-8F1E-4CA6-8CB9-D332C92058A4}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" guid="{F3A0AFD9-A5F6-47B0-B9B1-93C578E71F3C}" shapeId="0">
+    <comment ref="F1" authorId="0" guid="{5263D2AE-37B7-46DC-950C-5C2F03471985}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" guid="{F65F111C-31A2-46B7-B523-AD91A4A8CCCD}" shapeId="0">
+    <comment ref="G1" authorId="0" guid="{1F00F0EA-48F5-437D-9DAA-C9176A39691F}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" guid="{786887F7-A4CD-4F12-9237-36C0BA5FD11E}" shapeId="0">
+    <comment ref="H1" authorId="0" guid="{30F7526D-1DDD-4166-B382-04D13A4F742A}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" guid="{0230AF64-A559-4314-9D78-56FB26998881}" shapeId="0">
+    <comment ref="J1" authorId="0" guid="{64F44126-F4BB-4F5E-9680-324EC6254C7C}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -179,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="1" guid="{EAF9670C-BF70-4487-925D-8BA651790562}" shapeId="0">
+    <comment ref="L1" authorId="1" guid="{03D744C9-CD59-433B-86E8-4AF43AB38E77}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -205,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" guid="{4B8A231E-24AF-448E-A6CE-97380CF943E6}" shapeId="0">
+    <comment ref="M1" authorId="1" guid="{76EB66FD-008D-43BF-A70B-9ED53BF29CCC}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -231,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" guid="{B7BDF138-85B2-40C5-A14B-0311791DB1CA}" shapeId="0">
+    <comment ref="N1" authorId="1" guid="{69F8DEEF-88E3-469F-84D5-86DCA4D6B833}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -257,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="1" guid="{B767DBFA-327D-412A-9DE0-63128F6302CB}" shapeId="0">
+    <comment ref="O1" authorId="1" guid="{AC1CE88D-CFA3-4A46-958C-4320F2D45F08}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -283,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" guid="{7B83872C-57A7-4409-9199-F4231DA9ACB5}" shapeId="0">
+    <comment ref="P1" authorId="1" guid="{3099DCCE-A480-44AB-BDD7-489FBF3389DE}" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -309,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" guid="{C939A84F-49CF-4267-874C-6429EA63EE86}" shapeId="0">
+    <comment ref="Q1" authorId="1" guid="{5907216A-8367-437C-AA05-59256EF0BD39}" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -335,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" guid="{EB54849A-F509-409A-B305-12F67ABB7EDD}" shapeId="0">
+    <comment ref="R1" authorId="1" guid="{E30C0ABC-1FDD-464A-A265-F383B5EA1B5D}" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -361,7 +361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1" guid="{9B9D7869-FAE4-4653-A7A8-25A2474F8284}" shapeId="0">
+    <comment ref="S1" authorId="1" guid="{5628A306-682A-4EDF-B6B5-DCEF15B4D55C}" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -387,7 +387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1" guid="{C48E6EEA-9D03-4072-9B34-C5B31A1309CE}" shapeId="0">
+    <comment ref="T1" authorId="1" guid="{7DAED9C8-B4ED-43CC-9FB3-54648B7769F7}" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -413,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" guid="{B175D660-F9BE-4126-BBC2-1383E7B3F5C4}" shapeId="0">
+    <comment ref="U1" authorId="1" guid="{1361EF0C-C279-47C6-B700-79DEBBF41E2C}" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -439,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1" guid="{232F2948-76E8-4F3A-B2BB-39384C3C37ED}" shapeId="0">
+    <comment ref="V1" authorId="1" guid="{43E4F832-DB4C-4FAA-8097-177E11B8C413}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
       <text>
         <r>
           <rPr>
@@ -465,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1" guid="{1FC1C728-5106-4037-BA3D-92C1C50E51AA}" shapeId="0">
+    <comment ref="W1" authorId="1" guid="{7647BB95-D04A-41EA-B59B-DCDECCCD24CE}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
       <text>
         <r>
           <rPr>
@@ -491,7 +491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="1" guid="{FDE50646-E666-4233-909B-372465D23222}" shapeId="0">
+    <comment ref="X1" authorId="1" guid="{91FAD33E-469E-4BA7-BEE2-C0F6E8A045B7}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
       <text>
         <r>
           <rPr>
@@ -517,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1" guid="{DB3C8700-22C2-4CB1-BEE0-8E8D836A54C5}" shapeId="0">
+    <comment ref="Y1" authorId="1" guid="{FC53A88B-CBC2-4B40-B8D8-1DC204B197EA}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
       <text>
         <r>
           <rPr>
@@ -543,7 +543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="1" guid="{24A8262A-34F2-4B13-B5BE-50F6DD2DD290}" shapeId="0">
+    <comment ref="Z1" authorId="1" guid="{A82B9650-EAC7-4748-90EA-35453ED9D5D4}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
       <text>
         <r>
           <rPr>
@@ -569,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="1" guid="{6237D507-CD7E-41F9-9E0D-F00D2B4952C3}" shapeId="0">
+    <comment ref="AA1" authorId="1" guid="{C5C2B2B9-8461-4E8E-B78A-5EF2751B451F}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
       <text>
         <r>
           <rPr>
@@ -595,7 +595,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="1" guid="{370F0A60-3D8C-47F8-ABDA-780E9598A4AC}" shapeId="0">
+    <comment ref="AB1" authorId="1" guid="{CC0CD8FB-0818-460E-858E-2ABE9A9BC91F}" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
       <text>
         <r>
           <rPr>
@@ -626,13 +626,13 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dr. Johann Graf Lambsdorff</author>
     <author>Note</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" guid="{A62510E4-8F1E-4CA6-8CB9-D332C92058A4}" shapeId="0">
+    <comment ref="D1" authorId="0" guid="{5707E7BD-35E3-4F64-BD4B-25E4EA104ACD}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -655,7 +655,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" guid="{5263D2AE-37B7-46DC-950C-5C2F03471985}" shapeId="0">
+    <comment ref="F1" authorId="0" guid="{11F8E8DC-FE60-4A96-B140-A66419E95FF1}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -678,7 +678,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" guid="{1F00F0EA-48F5-437D-9DAA-C9176A39691F}" shapeId="0">
+    <comment ref="G1" authorId="0" guid="{F5D3D2B5-A29F-4C95-8E22-D515CF60523F}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -702,7 +702,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" guid="{30F7526D-1DDD-4166-B382-04D13A4F742A}" shapeId="0">
+    <comment ref="H1" authorId="0" guid="{12CCCAE4-0440-4275-A96A-7BCE27E918C1}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -726,7 +726,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" guid="{64F44126-F4BB-4F5E-9680-324EC6254C7C}" shapeId="0">
+    <comment ref="J1" authorId="0" guid="{612063AC-6FFB-44FD-ACEB-1765BC12F9AC}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -750,7 +750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" guid="{03D744C9-CD59-433B-86E8-4AF43AB38E77}" shapeId="0">
+    <comment ref="L1" authorId="1" guid="{A8AFE612-E2C3-465B-A512-5D5266B7A6AF}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -776,7 +776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" guid="{76EB66FD-008D-43BF-A70B-9ED53BF29CCC}" shapeId="0">
+    <comment ref="M1" authorId="1" guid="{7C1CB929-0849-47E2-AD75-B0A5F426C02D}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -802,7 +802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="1" guid="{69F8DEEF-88E3-469F-84D5-86DCA4D6B833}" shapeId="0">
+    <comment ref="N1" authorId="1" guid="{498AFD7A-71E0-40A2-9209-DA8ED2C5019A}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -828,7 +828,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" guid="{AC1CE88D-CFA3-4A46-958C-4320F2D45F08}" shapeId="0">
+    <comment ref="O1" authorId="1" guid="{BE0E33D6-CF8D-4D0C-9495-177E8082D93E}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -854,7 +854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" guid="{3099DCCE-A480-44AB-BDD7-489FBF3389DE}" shapeId="0">
+    <comment ref="P1" authorId="1" guid="{E319F543-6FAC-42C2-8D71-69612695984E}" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -880,7 +880,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" guid="{5907216A-8367-437C-AA05-59256EF0BD39}" shapeId="0">
+    <comment ref="Q1" authorId="1" guid="{80D4F9D4-8A36-486B-B9A6-9482C6D88AD8}" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -906,7 +906,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1" guid="{E30C0ABC-1FDD-464A-A265-F383B5EA1B5D}" shapeId="0">
+    <comment ref="R1" authorId="1" guid="{2A295F14-AC74-4DB3-80AA-B25444F0DCBA}" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -932,7 +932,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1" guid="{5628A306-682A-4EDF-B6B5-DCEF15B4D55C}" shapeId="0">
+    <comment ref="S1" authorId="1" guid="{1742F240-875E-4A49-8B2D-B6E59978A6CE}" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -958,7 +958,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" guid="{7DAED9C8-B4ED-43CC-9FB3-54648B7769F7}" shapeId="0">
+    <comment ref="T1" authorId="1" guid="{275C5D4E-FAD3-427E-BBB3-81DF7E16E16D}" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -984,7 +984,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1" guid="{1361EF0C-C279-47C6-B700-79DEBBF41E2C}" shapeId="0">
+    <comment ref="U1" authorId="1" guid="{84C140C1-FB98-4718-8AD3-FF4B5EC11A49}" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -1010,7 +1010,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1" guid="{43E4F832-DB4C-4FAA-8097-177E11B8C413}" shapeId="0">
+    <comment ref="V1" authorId="1" guid="{1EADD2A2-55A1-45BC-86BA-3FF2D3819674}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000010000000}">
       <text>
         <r>
           <rPr>
@@ -1036,7 +1036,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="1" guid="{7647BB95-D04A-41EA-B59B-DCDECCCD24CE}" shapeId="0">
+    <comment ref="W1" authorId="1" guid="{2E178E3A-EEB3-4F7C-B8C4-94920E281C01}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000011000000}">
       <text>
         <r>
           <rPr>
@@ -1062,7 +1062,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1" guid="{91FAD33E-469E-4BA7-BEE2-C0F6E8A045B7}" shapeId="0">
+    <comment ref="X1" authorId="1" guid="{2FC58AC1-9B46-414A-BF8A-6874D3DF7789}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000012000000}">
       <text>
         <r>
           <rPr>
@@ -1088,7 +1088,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="1" guid="{FC53A88B-CBC2-4B40-B8D8-1DC204B197EA}" shapeId="0">
+    <comment ref="Y1" authorId="1" guid="{CE18486D-BA76-4A90-A5F3-A5C11CE21034}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000013000000}">
       <text>
         <r>
           <rPr>
@@ -1114,7 +1114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="1" guid="{A82B9650-EAC7-4748-90EA-35453ED9D5D4}" shapeId="0">
+    <comment ref="Z1" authorId="1" guid="{0CB2721F-C9A7-47AB-BC2D-D6B3AEF91BA8}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000014000000}">
       <text>
         <r>
           <rPr>
@@ -1140,7 +1140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="1" guid="{C5C2B2B9-8461-4E8E-B78A-5EF2751B451F}" shapeId="0">
+    <comment ref="AA1" authorId="1" guid="{33D5A6E5-00B7-44D9-94C6-D25D243E432E}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000015000000}">
       <text>
         <r>
           <rPr>
@@ -1166,7 +1166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="1" guid="{CC0CD8FB-0818-460E-858E-2ABE9A9BC91F}" shapeId="0">
+    <comment ref="AB1" authorId="1" guid="{C1E6E898-CDB1-442A-8350-297202CDC1A2}" shapeId="0" xr:uid="{00000000-0006-0000-0300-000016000000}">
       <text>
         <r>
           <rPr>
@@ -1197,13 +1197,13 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dr. Johann Graf Lambsdorff</author>
     <author>Note</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" guid="{5707E7BD-35E3-4F64-BD4B-25E4EA104ACD}" shapeId="0">
+    <comment ref="D1" authorId="0" guid="{F6024514-44E1-47F5-AA7B-8C499AB5A58A}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1226,7 +1226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" guid="{11F8E8DC-FE60-4A96-B140-A66419E95FF1}" shapeId="0">
+    <comment ref="F1" authorId="0" guid="{4A46C98D-E51D-4B78-9144-5A796CCBA9C4}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1249,7 +1249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" guid="{F5D3D2B5-A29F-4C95-8E22-D515CF60523F}" shapeId="0">
+    <comment ref="G1" authorId="0" guid="{972F5470-CF00-4A1C-BA1D-6A4BE8EF1DB0}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1273,7 +1273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" guid="{12CCCAE4-0440-4275-A96A-7BCE27E918C1}" shapeId="0">
+    <comment ref="H1" authorId="0" guid="{9218C2BF-D5F4-413D-B9DB-2027840093C2}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1297,7 +1297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" guid="{612063AC-6FFB-44FD-ACEB-1765BC12F9AC}" shapeId="0">
+    <comment ref="J1" authorId="0" guid="{18023162-ED4F-423C-A849-978D5519E9AC}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1321,7 +1321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" guid="{A8AFE612-E2C3-465B-A512-5D5266B7A6AF}" shapeId="0">
+    <comment ref="L1" authorId="1" guid="{D1CD091A-9E2F-4673-BF39-EC315F88CE38}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1347,7 +1347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" guid="{7C1CB929-0849-47E2-AD75-B0A5F426C02D}" shapeId="0">
+    <comment ref="M1" authorId="1" guid="{BD5BF587-D8E6-441C-B43A-81C60413A069}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1373,7 +1373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="1" guid="{498AFD7A-71E0-40A2-9209-DA8ED2C5019A}" shapeId="0">
+    <comment ref="N1" authorId="1" guid="{EC9A5D8F-519D-45B2-B0EF-6EE28228ABA8}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1399,7 +1399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" guid="{BE0E33D6-CF8D-4D0C-9495-177E8082D93E}" shapeId="0">
+    <comment ref="O1" authorId="1" guid="{5DAF3FF1-1F6A-4E0B-A3AD-5FD1B690447B}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1425,7 +1425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" guid="{E319F543-6FAC-42C2-8D71-69612695984E}" shapeId="0">
+    <comment ref="P1" authorId="1" guid="{80F749B7-0634-4403-BA3D-5835AD830EF6}" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -1451,7 +1451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" guid="{80D4F9D4-8A36-486B-B9A6-9482C6D88AD8}" shapeId="0">
+    <comment ref="Q1" authorId="1" guid="{304FB76E-69A6-440A-82F5-B047327F009C}" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -1477,7 +1477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1" guid="{2A295F14-AC74-4DB3-80AA-B25444F0DCBA}" shapeId="0">
+    <comment ref="R1" authorId="1" guid="{5B6F4CF7-D7D3-4B2E-9005-316F6F4968FF}" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -1503,7 +1503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1" guid="{1742F240-875E-4A49-8B2D-B6E59978A6CE}" shapeId="0">
+    <comment ref="S1" authorId="1" guid="{25D26415-38EE-43E6-8686-43E9D1C599AD}" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -1529,7 +1529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" guid="{275C5D4E-FAD3-427E-BBB3-81DF7E16E16D}" shapeId="0">
+    <comment ref="T1" authorId="1" guid="{BC864EE5-7C72-4768-901C-241F3A481F96}" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -1555,7 +1555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1" guid="{84C140C1-FB98-4718-8AD3-FF4B5EC11A49}" shapeId="0">
+    <comment ref="U1" authorId="1" guid="{C264D265-16C0-43B7-90B5-97D22757C56D}" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -1581,7 +1581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1" guid="{1EADD2A2-55A1-45BC-86BA-3FF2D3819674}" shapeId="0">
+    <comment ref="V1" authorId="1" guid="{8E8EDEE3-3465-4865-B6C7-D8EFC3E068BC}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000010000000}">
       <text>
         <r>
           <rPr>
@@ -1607,7 +1607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="1" guid="{2E178E3A-EEB3-4F7C-B8C4-94920E281C01}" shapeId="0">
+    <comment ref="W1" authorId="1" guid="{C2338964-3485-4E78-80B5-33D2298FEB44}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000011000000}">
       <text>
         <r>
           <rPr>
@@ -1633,7 +1633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1" guid="{2FC58AC1-9B46-414A-BF8A-6874D3DF7789}" shapeId="0">
+    <comment ref="X1" authorId="1" guid="{24DA4E53-341B-4D49-8622-FF893F9C23E8}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000012000000}">
       <text>
         <r>
           <rPr>
@@ -1659,7 +1659,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="1" guid="{CE18486D-BA76-4A90-A5F3-A5C11CE21034}" shapeId="0">
+    <comment ref="Y1" authorId="1" guid="{BED42015-A562-48D1-A736-7CECEA12CECA}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000013000000}">
       <text>
         <r>
           <rPr>
@@ -1685,7 +1685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="1" guid="{0CB2721F-C9A7-47AB-BC2D-D6B3AEF91BA8}" shapeId="0">
+    <comment ref="Z1" authorId="1" guid="{2BC6439E-D0FE-4D5A-AF5B-0DF495A85C1B}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000014000000}">
       <text>
         <r>
           <rPr>
@@ -1711,7 +1711,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="1" guid="{33D5A6E5-00B7-44D9-94C6-D25D243E432E}" shapeId="0">
+    <comment ref="AA1" authorId="1" guid="{C5CA1F6B-742B-42CB-A662-4194F65025D7}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000015000000}">
       <text>
         <r>
           <rPr>
@@ -1737,7 +1737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="1" guid="{C1E6E898-CDB1-442A-8350-297202CDC1A2}" shapeId="0">
+    <comment ref="AB1" authorId="1" guid="{63287E38-944C-4D43-982D-058F865EBDB4}" shapeId="0" xr:uid="{00000000-0006-0000-0400-000016000000}">
       <text>
         <r>
           <rPr>
@@ -1768,13 +1768,13 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dr. Johann Graf Lambsdorff</author>
     <author>Note</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" guid="{F6024514-44E1-47F5-AA7B-8C499AB5A58A}" shapeId="0">
+    <comment ref="D1" authorId="0" guid="{12FBD202-A61F-42D2-A457-C7ED1298D94B}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1797,7 +1797,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" guid="{4A46C98D-E51D-4B78-9144-5A796CCBA9C4}" shapeId="0">
+    <comment ref="F1" authorId="0" guid="{A12BFD8C-3EEA-4686-9CD4-3E6F18822C24}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1820,7 +1820,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" guid="{972F5470-CF00-4A1C-BA1D-6A4BE8EF1DB0}" shapeId="0">
+    <comment ref="G1" authorId="0" guid="{F7516EF0-009B-4683-A9ED-EA7CBECE555F}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1844,7 +1844,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" guid="{9218C2BF-D5F4-413D-B9DB-2027840093C2}" shapeId="0">
+    <comment ref="H1" authorId="0" guid="{F6E30106-08A9-4362-8737-7A93B32D9601}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1868,7 +1868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" guid="{18023162-ED4F-423C-A849-978D5519E9AC}" shapeId="0">
+    <comment ref="J1" authorId="0" guid="{AE303983-E21B-42DD-AECE-A128F6E9BCEA}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1892,7 +1892,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" guid="{D1CD091A-9E2F-4673-BF39-EC315F88CE38}" shapeId="0">
+    <comment ref="L1" authorId="1" guid="{99B9FA4E-7E7B-4049-9034-F92D1A3AF42F}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1918,7 +1918,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" guid="{BD5BF587-D8E6-441C-B43A-81C60413A069}" shapeId="0">
+    <comment ref="M1" authorId="1" guid="{BF22FE8A-2711-4E56-821E-4BB43B094811}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1944,7 +1944,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="1" guid="{EC9A5D8F-519D-45B2-B0EF-6EE28228ABA8}" shapeId="0">
+    <comment ref="N1" authorId="1" guid="{0604B512-C961-4901-8AFE-D5185BD3697A}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1970,7 +1970,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" guid="{5DAF3FF1-1F6A-4E0B-A3AD-5FD1B690447B}" shapeId="0">
+    <comment ref="O1" authorId="1" guid="{48C02881-2497-4124-867B-A048C968ABB3}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1996,7 +1996,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" guid="{80F749B7-0634-4403-BA3D-5835AD830EF6}" shapeId="0">
+    <comment ref="P1" authorId="1" guid="{23EB5991-4D3E-482F-9F5A-BA2DD2DB0184}" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -2022,7 +2022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" guid="{304FB76E-69A6-440A-82F5-B047327F009C}" shapeId="0">
+    <comment ref="Q1" authorId="1" guid="{7E4E2426-F5B4-4C81-B8DD-9CB33F1F1169}" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -2048,7 +2048,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1" guid="{5B6F4CF7-D7D3-4B2E-9005-316F6F4968FF}" shapeId="0">
+    <comment ref="R1" authorId="1" guid="{02FC3EDA-29D7-47C2-9CAD-AAA91935F12B}" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -2074,7 +2074,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1" guid="{25D26415-38EE-43E6-8686-43E9D1C599AD}" shapeId="0">
+    <comment ref="S1" authorId="1" guid="{BF434BEB-FD3A-40D8-89E5-E8F0700FBD91}" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -2100,7 +2100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" guid="{BC864EE5-7C72-4768-901C-241F3A481F96}" shapeId="0">
+    <comment ref="T1" authorId="1" guid="{04E26416-8C8F-4824-BFF7-781C9BEDC47B}" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -2126,7 +2126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1" guid="{C264D265-16C0-43B7-90B5-97D22757C56D}" shapeId="0">
+    <comment ref="U1" authorId="1" guid="{5F88739F-EDE1-46C8-A264-553E5A12FCBD}" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -2152,7 +2152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1" guid="{8E8EDEE3-3465-4865-B6C7-D8EFC3E068BC}" shapeId="0">
+    <comment ref="V1" authorId="1" guid="{7D25E586-B705-4700-AC3A-D3622B12CB4B}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000010000000}">
       <text>
         <r>
           <rPr>
@@ -2178,7 +2178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="1" guid="{C2338964-3485-4E78-80B5-33D2298FEB44}" shapeId="0">
+    <comment ref="W1" authorId="1" guid="{09ECE592-7C6D-4063-934D-646A2C75C21F}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000011000000}">
       <text>
         <r>
           <rPr>
@@ -2204,7 +2204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1" guid="{24DA4E53-341B-4D49-8622-FF893F9C23E8}" shapeId="0">
+    <comment ref="X1" authorId="1" guid="{412E17AB-BEB3-47F9-A183-371669DCA748}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000012000000}">
       <text>
         <r>
           <rPr>
@@ -2230,7 +2230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="1" guid="{BED42015-A562-48D1-A736-7CECEA12CECA}" shapeId="0">
+    <comment ref="Y1" authorId="1" guid="{3F7D03B7-0B4C-4F60-94A9-B39771BBDAFA}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000013000000}">
       <text>
         <r>
           <rPr>
@@ -2256,7 +2256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="1" guid="{2BC6439E-D0FE-4D5A-AF5B-0DF495A85C1B}" shapeId="0">
+    <comment ref="Z1" authorId="1" guid="{A048B4E2-CC27-44DA-807E-907599F8A0D3}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000014000000}">
       <text>
         <r>
           <rPr>
@@ -2282,7 +2282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="1" guid="{C5CA1F6B-742B-42CB-A662-4194F65025D7}" shapeId="0">
+    <comment ref="AA1" authorId="1" guid="{EBE50093-3B55-475B-B94F-6CC2C7C187CA}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000015000000}">
       <text>
         <r>
           <rPr>
@@ -2308,7 +2308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="1" guid="{63287E38-944C-4D43-982D-058F865EBDB4}" shapeId="0">
+    <comment ref="AB1" authorId="1" guid="{1E2E2E59-F917-47B3-8660-F474C088D841}" shapeId="0" xr:uid="{00000000-0006-0000-0500-000016000000}">
       <text>
         <r>
           <rPr>
@@ -2339,13 +2339,13 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dr. Johann Graf Lambsdorff</author>
     <author>Note</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" guid="{12FBD202-A61F-42D2-A457-C7ED1298D94B}" shapeId="0">
+    <comment ref="D1" authorId="0" guid="{74464AE8-6013-4F60-B454-3D7C8EFA8440}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -2368,7 +2368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" guid="{A12BFD8C-3EEA-4686-9CD4-3E6F18822C24}" shapeId="0">
+    <comment ref="F1" authorId="0" guid="{E3631ABD-791B-4AE7-A80F-22FBEB65DEA2}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -2391,7 +2391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" guid="{F7516EF0-009B-4683-A9ED-EA7CBECE555F}" shapeId="0">
+    <comment ref="G1" authorId="0" guid="{A164C459-AE49-4814-83C5-AFB29F23AD17}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -2415,7 +2415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" guid="{F6E30106-08A9-4362-8737-7A93B32D9601}" shapeId="0">
+    <comment ref="H1" authorId="0" guid="{CC13551D-3C5D-47D1-91E3-27556DB0EE14}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -2439,7 +2439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" guid="{AE303983-E21B-42DD-AECE-A128F6E9BCEA}" shapeId="0">
+    <comment ref="J1" authorId="0" guid="{CA2FC23C-A08B-4528-AAB2-DFA49572885D}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -2463,7 +2463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" guid="{99B9FA4E-7E7B-4049-9034-F92D1A3AF42F}" shapeId="0">
+    <comment ref="L1" authorId="1" guid="{E240FF3C-07AD-4AEC-BFDB-59CC1F6CECEA}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
       <text>
         <r>
           <rPr>
@@ -2489,7 +2489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" guid="{BF22FE8A-2711-4E56-821E-4BB43B094811}" shapeId="0">
+    <comment ref="M1" authorId="1" guid="{E4849B74-0FBE-4C87-A648-B8E78F67CCB4}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
       <text>
         <r>
           <rPr>
@@ -2515,7 +2515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="1" guid="{0604B512-C961-4901-8AFE-D5185BD3697A}" shapeId="0">
+    <comment ref="N1" authorId="1" guid="{D88299E6-7213-4AA1-928C-8164491906BC}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000008000000}">
       <text>
         <r>
           <rPr>
@@ -2541,7 +2541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" guid="{48C02881-2497-4124-867B-A048C968ABB3}" shapeId="0">
+    <comment ref="O1" authorId="1" guid="{E617CB9F-1760-498D-901F-5AC1C0961CF6}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000009000000}">
       <text>
         <r>
           <rPr>
@@ -2567,7 +2567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" guid="{23EB5991-4D3E-482F-9F5A-BA2DD2DB0184}" shapeId="0">
+    <comment ref="P1" authorId="1" guid="{B9CE03FB-20F9-4DBF-9D03-CAC4C52F68E0}" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -2593,7 +2593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" guid="{7E4E2426-F5B4-4C81-B8DD-9CB33F1F1169}" shapeId="0">
+    <comment ref="Q1" authorId="1" guid="{69E93C0B-C044-445E-B77B-A32A74EC90FD}" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -2619,7 +2619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1" guid="{02FC3EDA-29D7-47C2-9CAD-AAA91935F12B}" shapeId="0">
+    <comment ref="R1" authorId="1" guid="{19B4113A-99CE-437F-9DB3-37442EBED9DA}" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -2645,7 +2645,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1" guid="{BF434BEB-FD3A-40D8-89E5-E8F0700FBD91}" shapeId="0">
+    <comment ref="S1" authorId="1" guid="{87110F63-A1C0-4DDE-9ED6-98E1E9F681FF}" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -2671,7 +2671,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" guid="{04E26416-8C8F-4824-BFF7-781C9BEDC47B}" shapeId="0">
+    <comment ref="T1" authorId="1" guid="{D29CE886-84E6-4FF5-A379-5A18DC348467}" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -2697,7 +2697,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1" guid="{5F88739F-EDE1-46C8-A264-553E5A12FCBD}" shapeId="0">
+    <comment ref="U1" authorId="1" guid="{E9C1379A-E5A4-4644-9E08-6D7AADD5B007}" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -2723,7 +2723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1" guid="{7D25E586-B705-4700-AC3A-D3622B12CB4B}" shapeId="0">
+    <comment ref="V1" authorId="1" guid="{E7AC81F1-B528-41AF-A06F-07C87042A270}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000010000000}">
       <text>
         <r>
           <rPr>
@@ -2749,7 +2749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="1" guid="{09ECE592-7C6D-4063-934D-646A2C75C21F}" shapeId="0">
+    <comment ref="W1" authorId="1" guid="{F2E23C15-02DD-4453-B293-BF252D1F2CD9}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000011000000}">
       <text>
         <r>
           <rPr>
@@ -2775,7 +2775,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1" guid="{412E17AB-BEB3-47F9-A183-371669DCA748}" shapeId="0">
+    <comment ref="X1" authorId="1" guid="{60E01F32-A55D-4366-9CE1-01DB034CDE29}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000012000000}">
       <text>
         <r>
           <rPr>
@@ -2801,7 +2801,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="1" guid="{3F7D03B7-0B4C-4F60-94A9-B39771BBDAFA}" shapeId="0">
+    <comment ref="Y1" authorId="1" guid="{3154303D-F189-426B-B53D-86E6171E8CB3}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000013000000}">
       <text>
         <r>
           <rPr>
@@ -2827,7 +2827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="1" guid="{A048B4E2-CC27-44DA-807E-907599F8A0D3}" shapeId="0">
+    <comment ref="Z1" authorId="1" guid="{D46ED168-E126-44D5-9A82-8D826811337F}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000014000000}">
       <text>
         <r>
           <rPr>
@@ -2853,7 +2853,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="1" guid="{EBE50093-3B55-475B-B94F-6CC2C7C187CA}" shapeId="0">
+    <comment ref="AA1" authorId="1" guid="{34C99BDE-CBB4-480A-B973-CF259E09D927}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000015000000}">
       <text>
         <r>
           <rPr>
@@ -2879,7 +2879,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="1" guid="{1E2E2E59-F917-47B3-8660-F474C088D841}" shapeId="0">
+    <comment ref="AB1" authorId="1" guid="{9A39C3E8-40BC-4C6B-A1BA-18A97AC355BB}" shapeId="0" xr:uid="{00000000-0006-0000-0600-000016000000}">
       <text>
         <r>
           <rPr>
@@ -2910,13 +2910,13 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dr. Johann Graf Lambsdorff</author>
     <author>Note</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" guid="{74464AE8-6013-4F60-B454-3D7C8EFA8440}" shapeId="0">
+    <comment ref="D1" authorId="0" guid="{D8F462BB-42EF-4EB1-BE1D-9CE4548A11E2}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -2939,7 +2939,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" guid="{E3631ABD-791B-4AE7-A80F-22FBEB65DEA2}" shapeId="0">
+    <comment ref="F1" authorId="0" guid="{6C118D7E-C2AE-4553-BB59-196ADC0F401E}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000002000000}">
       <text>
         <r>
           <rPr>
@@ -2962,7 +2962,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" guid="{A164C459-AE49-4814-83C5-AFB29F23AD17}" shapeId="0">
+    <comment ref="G1" authorId="0" guid="{AA213730-492B-4815-9496-D97C27A0F953}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000003000000}">
       <text>
         <r>
           <rPr>
@@ -2986,7 +2986,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" guid="{CC13551D-3C5D-47D1-91E3-27556DB0EE14}" shapeId="0">
+    <comment ref="H1" authorId="0" guid="{B7BC87CA-F70C-4C06-AE47-26C4D3BF06CE}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000004000000}">
       <text>
         <r>
           <rPr>
@@ -3010,7 +3010,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" guid="{CA2FC23C-A08B-4528-AAB2-DFA49572885D}" shapeId="0">
+    <comment ref="J1" authorId="0" guid="{946C0230-3F1F-44A2-B22E-292632CA7364}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000005000000}">
       <text>
         <r>
           <rPr>
@@ -3034,7 +3034,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" guid="{E240FF3C-07AD-4AEC-BFDB-59CC1F6CECEA}" shapeId="0">
+    <comment ref="L1" authorId="1" guid="{B5738376-3ABC-4C45-9B3D-858F0A9D5586}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000006000000}">
       <text>
         <r>
           <rPr>
@@ -3060,7 +3060,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" guid="{E4849B74-0FBE-4C87-A648-B8E78F67CCB4}" shapeId="0">
+    <comment ref="M1" authorId="1" guid="{3A7545BA-C9D5-4DDB-9C39-65A548F7AE4A}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000007000000}">
       <text>
         <r>
           <rPr>
@@ -3086,7 +3086,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="1" guid="{D88299E6-7213-4AA1-928C-8164491906BC}" shapeId="0">
+    <comment ref="N1" authorId="1" guid="{953DE722-91D9-4908-B94F-027137C356C1}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000008000000}">
       <text>
         <r>
           <rPr>
@@ -3112,7 +3112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" guid="{E617CB9F-1760-498D-901F-5AC1C0961CF6}" shapeId="0">
+    <comment ref="O1" authorId="1" guid="{96DA73E4-6D6B-4983-A5FC-588F8A40D92A}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000009000000}">
       <text>
         <r>
           <rPr>
@@ -3138,7 +3138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" guid="{B9CE03FB-20F9-4DBF-9D03-CAC4C52F68E0}" shapeId="0">
+    <comment ref="P1" authorId="1" guid="{8B081140-6330-4B20-9D14-19F7640D0543}" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -3164,7 +3164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" guid="{69E93C0B-C044-445E-B77B-A32A74EC90FD}" shapeId="0">
+    <comment ref="Q1" authorId="1" guid="{DF0DB4FC-B848-48AF-BD20-0376AAA81FBD}" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -3190,7 +3190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1" guid="{19B4113A-99CE-437F-9DB3-37442EBED9DA}" shapeId="0">
+    <comment ref="R1" authorId="1" guid="{5B114356-4A63-4A1C-A499-999DE2B8F70E}" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -3216,7 +3216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1" guid="{87110F63-A1C0-4DDE-9ED6-98E1E9F681FF}" shapeId="0">
+    <comment ref="S1" authorId="1" guid="{BE2DFFE6-908E-4D53-90BD-32BE3AAE5200}" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -3242,7 +3242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" guid="{D29CE886-84E6-4FF5-A379-5A18DC348467}" shapeId="0">
+    <comment ref="T1" authorId="1" guid="{F9CDFFAB-6751-4419-9DD1-B10E912B3E44}" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -3268,7 +3268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1" guid="{E9C1379A-E5A4-4644-9E08-6D7AADD5B007}" shapeId="0">
+    <comment ref="U1" authorId="1" guid="{4D604076-B31F-40A9-B7AD-458DA38149EB}" shapeId="0" xr:uid="{00000000-0006-0000-0700-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -3294,7 +3294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1" guid="{E7AC81F1-B528-41AF-A06F-07C87042A270}" shapeId="0">
+    <comment ref="V1" authorId="1" guid="{2D3235E0-4FC1-48DA-9FC6-6B0D9ED54D0E}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000010000000}">
       <text>
         <r>
           <rPr>
@@ -3320,7 +3320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="1" guid="{F2E23C15-02DD-4453-B293-BF252D1F2CD9}" shapeId="0">
+    <comment ref="W1" authorId="1" guid="{515DC1ED-D956-4B2B-B1D2-51B42655AA25}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000011000000}">
       <text>
         <r>
           <rPr>
@@ -3346,7 +3346,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1" guid="{60E01F32-A55D-4366-9CE1-01DB034CDE29}" shapeId="0">
+    <comment ref="X1" authorId="1" guid="{D42F5E47-09C1-401C-8175-8274E1D4B76F}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000012000000}">
       <text>
         <r>
           <rPr>
@@ -3372,7 +3372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="1" guid="{3154303D-F189-426B-B53D-86E6171E8CB3}" shapeId="0">
+    <comment ref="Y1" authorId="1" guid="{A3DC54F2-BAE9-4483-8796-76E9ADB15E9E}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000013000000}">
       <text>
         <r>
           <rPr>
@@ -3398,7 +3398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="1" guid="{D46ED168-E126-44D5-9A82-8D826811337F}" shapeId="0">
+    <comment ref="Z1" authorId="1" guid="{F4DD7D93-95B8-41D2-9A3C-F40CC1D56F23}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000014000000}">
       <text>
         <r>
           <rPr>
@@ -3424,7 +3424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="1" guid="{34C99BDE-CBB4-480A-B973-CF259E09D927}" shapeId="0">
+    <comment ref="AA1" authorId="1" guid="{81E639F3-7104-4DAD-BB4D-B021A6EA0452}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000015000000}">
       <text>
         <r>
           <rPr>
@@ -3450,578 +3450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="1" guid="{9A39C3E8-40BC-4C6B-A1BA-18A97AC355BB}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-World Justice Project Rule of Law Index
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Dr. Johann Graf Lambsdorff</author>
-    <author>Note</author>
-  </authors>
-  <commentList>
-    <comment ref="D1" authorId="0" guid="{D8F462BB-42EF-4EB1-BE1D-9CE4548A11E2}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">CPI 2010 Score -  </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>relates to the degree to which corruption is perceived to exist among public officials and politicians by business people and country analysts. Score ranges between 10 (highly clean) and 0 (highly corrupt).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" guid="{6C118D7E-C2AE-4553-BB59-196ADC0F401E}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Surveys Used -  </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Reflects the number of surveys or assessments used to calculate the CPI score for each country. In 2010  there were 13 surveys and expert assessments used and at least 3 were required for a country to be included in the CPI.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" guid="{AA213730-492B-4815-9496-D97C27A0F953}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Standard Deviation - 
-   </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>indicates differences in the values of the sources. The smaller the Standard Deviation the greater the agreement in the valuation of the sources.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" guid="{B7BC87CA-F70C-4C06-AE47-26C4D3BF06CE}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">High-Low Range  - 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">   provides the highest and lowest values of the sources. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" guid="{946C0230-3F1F-44A2-B22E-292632CA7364}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The confidence range -
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">    provides a range of possible values of the CPI score. This reflects how a country's score may vary, depending on measurement precision. Nominally, with 5 percent probability the score is above this range and with another 5 percent it is below. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="1" guid="{B5738376-3ABC-4C45-9B3D-858F0A9D5586}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-African Development Bank Governance Ratings
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="1" guid="{3A7545BA-C9D5-4DDB-9C39-65A548F7AE4A}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Asian Development Bank Country Performance Assessment
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="1" guid="{953DE722-91D9-4908-B94F-027137C356C1}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Bertelsmann Foundation Sustainable Governance Indicators
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="1" guid="{96DA73E4-6D6B-4983-A5FC-588F8A40D92A}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Bertelsmann Foundation Transformation Index 
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P1" authorId="1" guid="{8B081140-6330-4B20-9D14-19F7640D0543}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Economist Intelligence Unit Country Risk Assessment
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q1" authorId="1" guid="{DF0DB4FC-B848-48AF-BD20-0376AAA81FBD}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Freedom House Nations in Transit
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R1" authorId="1" guid="{5B114356-4A63-4A1C-A499-999DE2B8F70E}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Global Insight Country Risk Ratings  
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S1" authorId="1" guid="{BE2DFFE6-908E-4D53-90BD-32BE3AAE5200}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-IMD World Competitiveness Year Book 2010  
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T1" authorId="1" guid="{F9CDFFAB-6751-4419-9DD1-B10E912B3E44}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-IMD World Competitiveness Year Book 2011  
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U1" authorId="1" guid="{4D604076-B31F-40A9-B7AD-458DA38149EB}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Political and Economic Risk Consultancy 2010
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="1" guid="{2D3235E0-4FC1-48DA-9FC6-6B0D9ED54D0E}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Political and Economic Risk Consultancy 2011
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W1" authorId="1" guid="{515DC1ED-D956-4B2B-B1D2-51B42655AA25}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Political Risk Services International Country Risk Guide
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X1" authorId="1" guid="{D42F5E47-09C1-401C-8175-8274E1D4B76F}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Transparency International Bribe Payers Survey
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Y1" authorId="1" guid="{A3DC54F2-BAE9-4483-8796-76E9ADB15E9E}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-World Bank Country Performance and Institutional Assessment
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z1" authorId="1" guid="{F4DD7D93-95B8-41D2-9A3C-F40CC1D56F23}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-World Economic Forum Executive Opinion Survey (EOS) 2010
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA1" authorId="1" guid="{81E639F3-7104-4DAD-BB4D-B021A6EA0452}" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Note:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-World Economic Forum Executive Opinion Survey (EOS) 2011
-Code
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB1" authorId="1" guid="{0A286554-90BA-4148-B9A6-B0AA7B37A7AA}" shapeId="0">
+    <comment ref="AB1" authorId="1" guid="{0A286554-90BA-4148-B9A6-B0AA7B37A7AA}" shapeId="0" xr:uid="{00000000-0006-0000-0700-000016000000}">
       <text>
         <r>
           <rPr>
@@ -4912,9 +4341,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -5236,7 +4665,7 @@
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5270,49 +4699,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5321,16 +4756,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard_cpi-mp-be-stats" xfId="1"/>
+    <cellStyle name="Standard_cpi-mp-be-stats" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -5359,8 +4788,36 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CF2C14D1-757A-4DB4-9673-52D1D89AA6F2}" diskRevisions="1" revisionId="38" version="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8E110462-CFBA-4354-A864-CB98D874179D}" diskRevisions="1" revisionId="38" version="4">
   <header guid="{CF2C14D1-757A-4DB4-9673-52D1D89AA6F2}" dateTime="2020-09-20T12:37:22" maxSheetId="11" userName="Aidan Brown" r:id="rId11">
+    <sheetIdMap count="10">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="9"/>
+      <sheetId val="10"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{41213027-BF20-48D0-A797-7065459653D0}" dateTime="2020-09-20T13:08:22" maxSheetId="11" userName="Aidan Brown" r:id="rId12">
+    <sheetIdMap count="10">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="9"/>
+      <sheetId val="10"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8E110462-CFBA-4354-A864-CB98D874179D}" dateTime="2020-09-20T13:16:32" maxSheetId="11" userName="Aidan Brown" r:id="rId13">
     <sheetIdMap count="10">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -5377,14 +4834,50 @@
 </headers>
 </file>
 
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" action="delete"/>
+  <rcv guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" action="add"/>
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcmt sheetId="2" cell="C1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Dr. Johann Graf Lambsdorff"/>
+  <rcmt sheetId="2" cell="E1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Dr. Johann Graf Lambsdorff"/>
+  <rcmt sheetId="2" cell="F1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Dr. Johann Graf Lambsdorff"/>
+  <rcmt sheetId="2" cell="G1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" hiddenColumn="1" author="Dr. Johann Graf Lambsdorff"/>
+  <rcmt sheetId="2" cell="I1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Dr. Johann Graf Lambsdorff"/>
+  <rcmt sheetId="2" cell="K1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="L1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="M1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="N1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="O1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="P1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="Q1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="R1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="S1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="T1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="U1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="V1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="W1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="X1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="Y1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="Z1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+  <rcmt sheetId="2" cell="AA1" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Note"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{8E110462-CFBA-4354-A864-CB98D874179D}" name="Aidan Brown" id="-292380556" dateTime="2020-09-20T13:12:26"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5683,7 +5176,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S184"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -11168,11 +10661,6 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" state="hidden" topLeftCell="A2">
-      <selection activeCell="C46" sqref="C46"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
     <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" state="hidden" showRuler="0" topLeftCell="A2">
       <selection activeCell="C46" sqref="C46"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11198,6 +10686,11 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
+    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" state="hidden" topLeftCell="A2">
+      <selection activeCell="C46" sqref="C46"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11206,7 +10699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:R212"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -17573,11 +17066,6 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" state="hidden" topLeftCell="D1">
-      <selection activeCell="L2" sqref="L2"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
     <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" state="hidden" showRuler="0" topLeftCell="D1">
       <selection activeCell="L2" sqref="L2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -17603,6 +17091,11 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
+    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" state="hidden" topLeftCell="D1">
+      <selection activeCell="L2" sqref="L2"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -17611,11 +17104,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17629,91 +17122,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="34" t="s">
+      <c r="H1" s="37"/>
+      <c r="I1" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="37" t="s">
+      <c r="J1" s="38"/>
+      <c r="K1" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="V1" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="W1" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="X1" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="Y1" s="39" t="s">
+      <c r="Y1" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="Z1" s="39" t="s">
+      <c r="Z1" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="AA1" s="39" t="s">
+      <c r="AA1" s="34" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="18" t="s">
         <v>271</v>
       </c>
@@ -17726,23 +17219,23 @@
       <c r="J2" s="27" t="s">
         <v>273</v>
       </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
       <c r="AC2" t="s">
         <v>284</v>
       </c>
@@ -29335,28 +28828,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
+    <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" showRuler="0">
       <selection activeCell="H2" sqref="H2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" showRuler="0">
-      <selection activeCell="H2" sqref="H2"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
     <customSheetView guid="{7279341D-4A93-45C7-96BD-49257ECF5365}" showRuler="0">
       <selection activeCell="AA1" sqref="AA1:AA2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
     <customSheetView guid="{D1F0CD4F-E178-400D-8129-E15FD202F118}" showRuler="0">
       <selection activeCell="AB17" sqref="AB17"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
     <customSheetView guid="{62F7D542-8BF7-4494-AF3C-DE037CC9A023}" showRuler="0" topLeftCell="A148">
@@ -29366,6 +28853,12 @@
     </customSheetView>
     <customSheetView guid="{74EB1777-F5EA-4A6C-95F8-C57AD2099046}" showRuler="0">
       <selection activeCell="H2" sqref="H2"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
+      <selection activeCell="O1" sqref="O1:O2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
       <headerFooter alignWithMargins="0"/>
@@ -29379,11 +28872,6 @@
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
@@ -29391,23 +28879,27 @@
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -29425,97 +28917,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="37" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="V1" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="W1" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="X1" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="Y1" s="39" t="s">
+      <c r="Y1" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="Z1" s="39" t="s">
+      <c r="Z1" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="AA1" s="39" t="s">
+      <c r="AA1" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="AB1" s="39" t="s">
+      <c r="AB1" s="34" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="18" t="s">
         <v>271</v>
       </c>
@@ -29528,23 +29020,23 @@
       <c r="K2" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
       <c r="AD2" t="s">
         <v>284</v>
       </c>
@@ -31637,11 +31129,6 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
-      <selection activeCell="I2" sqref="I2"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
     <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" showRuler="0">
       <selection activeCell="I2" sqref="I2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -31667,11 +31154,13 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
+    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
+      <selection activeCell="I2" sqref="I2"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="26">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
@@ -31689,12 +31178,15 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -31704,7 +31196,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -31722,97 +31214,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="37" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="V1" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="W1" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="X1" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="Y1" s="39" t="s">
+      <c r="Y1" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="Z1" s="39" t="s">
+      <c r="Z1" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="AA1" s="39" t="s">
+      <c r="AA1" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="AB1" s="39" t="s">
+      <c r="AB1" s="34" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="18" t="s">
         <v>271</v>
       </c>
@@ -31825,23 +31317,23 @@
       <c r="K2" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
       <c r="AD2" t="s">
         <v>284</v>
       </c>
@@ -34195,11 +33687,6 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
-      <selection activeCell="I2" sqref="I2"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
     <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" showRuler="0">
       <selection activeCell="I2" sqref="I2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -34225,11 +33712,13 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
+    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
+      <selection activeCell="I2" sqref="I2"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="26">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
@@ -34247,12 +33736,15 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -34262,7 +33754,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34280,97 +33772,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="37" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="V1" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="W1" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="X1" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="Y1" s="39" t="s">
+      <c r="Y1" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="Z1" s="39" t="s">
+      <c r="Z1" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="AA1" s="39" t="s">
+      <c r="AA1" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="AB1" s="39" t="s">
+      <c r="AB1" s="34" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="18" t="s">
         <v>271</v>
       </c>
@@ -34383,23 +33875,23 @@
       <c r="K2" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
       <c r="AD2" t="s">
         <v>284</v>
       </c>
@@ -35736,11 +35228,6 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
-      <selection activeCell="I2" sqref="I2"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
     <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" showRuler="0">
       <selection activeCell="I2" sqref="I2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -35766,11 +35253,13 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
+    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
+      <selection activeCell="I2" sqref="I2"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="26">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
@@ -35788,12 +35277,15 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -35803,7 +35295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -35821,97 +35313,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="37" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="V1" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="W1" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="X1" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="Y1" s="39" t="s">
+      <c r="Y1" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="Z1" s="39" t="s">
+      <c r="Z1" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="AA1" s="39" t="s">
+      <c r="AA1" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="AB1" s="39" t="s">
+      <c r="AB1" s="34" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="18" t="s">
         <v>271</v>
       </c>
@@ -35924,23 +35416,23 @@
       <c r="K2" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
       <c r="AD2" t="s">
         <v>284</v>
       </c>
@@ -38041,11 +37533,6 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
-      <selection activeCell="I2" sqref="I2"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
     <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" showRuler="0">
       <selection activeCell="I2" sqref="I2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -38071,11 +37558,13 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
+    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
+      <selection activeCell="I2" sqref="I2"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="26">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
@@ -38093,12 +37582,15 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -38108,7 +37600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -38126,97 +37618,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="37" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="V1" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="W1" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="X1" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="Y1" s="39" t="s">
+      <c r="Y1" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="Z1" s="39" t="s">
+      <c r="Z1" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="AA1" s="39" t="s">
+      <c r="AA1" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="AB1" s="39" t="s">
+      <c r="AB1" s="34" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="18" t="s">
         <v>271</v>
       </c>
@@ -38229,23 +37721,23 @@
       <c r="K2" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
       <c r="AD2" t="s">
         <v>284</v>
       </c>
@@ -39426,11 +38918,6 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
-      <selection activeCell="I2" sqref="I2"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
     <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" showRuler="0">
       <selection activeCell="I2" sqref="I2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -39456,11 +38943,13 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
+    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
+      <selection activeCell="I2" sqref="I2"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="26">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
@@ -39478,12 +38967,15 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -39493,7 +38985,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39511,97 +39003,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="37" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="V1" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="W1" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="X1" s="39" t="s">
+      <c r="X1" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="Y1" s="39" t="s">
+      <c r="Y1" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="Z1" s="39" t="s">
+      <c r="Z1" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="AA1" s="39" t="s">
+      <c r="AA1" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="AB1" s="39" t="s">
+      <c r="AB1" s="34" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="18" t="s">
         <v>271</v>
       </c>
@@ -39614,23 +39106,23 @@
       <c r="K2" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
       <c r="AD2" t="s">
         <v>284</v>
       </c>
@@ -42742,11 +42234,6 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
-      <selection activeCell="I2" sqref="I2"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
     <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" showRuler="0">
       <selection activeCell="I2" sqref="I2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -42772,11 +42259,13 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
+    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}">
+      <selection activeCell="I2" sqref="I2"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="26">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
@@ -42794,12 +42283,15 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -42809,7 +42301,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S213"/>
   <sheetViews>
     <sheetView topLeftCell="A123" workbookViewId="0">
@@ -57755,11 +57247,6 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" state="hidden" topLeftCell="A123">
-      <selection activeCell="B70" sqref="B70"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
     <customSheetView guid="{0B59833F-5AE9-46E5-998B-A2C6554FCA70}" state="hidden" showRuler="0" topLeftCell="A123">
       <selection activeCell="B70" sqref="B70"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -57785,6 +57272,11 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
+    <customSheetView guid="{DD87A1E5-C277-4B9A-9C1E-660DC3647D12}" state="hidden" topLeftCell="A123">
+      <selection activeCell="B70" sqref="B70"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:S184">

</xml_diff>